<commit_message>
Override Dupes Clause (#37)
* feat: move importing json encounters from init to separate function

* feat: json imported encounters removed from notes and are initialized as pass 0

* fix: importEncounterJSON absolute path

* feat: remove encounter columns from df if they can no longer be accessed

* add mutually exclusive group to parser

* feat: only route if the correct argument is provided

* fix: importEncountersJSON recurses properly

* add honey tree encounter data to Game

* feat: honey trees are now all recorded when a group containing honey trees is pulled in checkDuplicates

* fix: rename route in ss, fix filtering in internal honey tree assignment

* fix: failed encounter routes are filtered from the df and no longer assigned an encounter

* fix: import json encounters ignores failed routes when building assignMe

* fix: changed Mr. Mime back to Mr-Mime for pokeapi parsing

* update gitignore to ignore all user json files
</commit_message>
<xml_diff>
--- a/EncounterRoutingNRotM/NRotMAugust2024.xlsx
+++ b/EncounterRoutingNRotM/NRotMAugust2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f30cbaf81810b05/Documents/Programming/pokemonDataTools/EncounterRoutingNRotM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gil\OneDrive\Documents\Programming\pokemonDataTools\EncounterRoutingNRotM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{CBC81FE4-5CCE-4303-970D-0617F9213FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC2A7B2-D5BA-49A4-A988-3C4C81434B32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EA599C-2551-4C49-BA17-9CD4EC78431C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -1012,9 +1012,6 @@
     <t>Ravaged Path</t>
   </si>
   <si>
-    <t>Floroama Meadow</t>
-  </si>
-  <si>
     <t>Death Counts (DO NOT TOUCH)</t>
   </si>
   <si>
@@ -2210,6 +2207,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Floaroma Meadow</t>
   </si>
 </sst>
 </file>
@@ -4794,10 +4794,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -7307,8 +7303,8 @@
   </sheetPr>
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8189,7 +8185,7 @@
       <c r="G17" s="136"/>
       <c r="H17" s="51"/>
       <c r="I17" s="42" t="s">
-        <v>190</v>
+        <v>478</v>
       </c>
       <c r="J17" s="43"/>
       <c r="K17" s="44" t="e">
@@ -8347,7 +8343,7 @@
     <row r="20" spans="1:24" ht="21">
       <c r="A20" s="30"/>
       <c r="B20" s="198" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="134"/>
       <c r="D20" s="30"/>
@@ -8356,7 +8352,7 @@
       <c r="G20" s="30"/>
       <c r="H20" s="51"/>
       <c r="I20" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J20" s="43"/>
       <c r="K20" s="44" t="e">
@@ -8404,14 +8400,14 @@
     <row r="21" spans="1:24" ht="21">
       <c r="A21" s="30"/>
       <c r="B21" s="61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C21" s="62">
         <f>COUNTIF($G$25:$G67, "B")</f>
         <v>0</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="62">
         <f>COUNTIF($D$25:$D67, "H")</f>
@@ -8421,7 +8417,7 @@
       <c r="G21" s="30"/>
       <c r="H21" s="51"/>
       <c r="I21" s="42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J21" s="43"/>
       <c r="K21" s="44" t="e">
@@ -8469,14 +8465,14 @@
     <row r="22" spans="1:24" ht="21">
       <c r="A22" s="30"/>
       <c r="B22" s="61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C22" s="62">
         <f>COUNTIF($G$25:$G67, "M")</f>
         <v>0</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E22" s="62">
         <f>COUNTIF($D$25:$D67, "S")</f>
@@ -8486,7 +8482,7 @@
       <c r="G22" s="30"/>
       <c r="H22" s="51"/>
       <c r="I22" s="53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="55" t="e">
@@ -8538,14 +8534,14 @@
     <row r="23" spans="1:24" ht="21">
       <c r="A23" s="30"/>
       <c r="B23" s="61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" s="63">
         <f>COUNTIF($G$25:$G67, "F/S")</f>
         <v>0</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E23" s="62">
         <f>COUNTIF($D$25:$D67, "L")</f>
@@ -8555,7 +8551,7 @@
       <c r="G23" s="30"/>
       <c r="H23" s="51"/>
       <c r="I23" s="42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J23" s="43"/>
       <c r="K23" s="44" t="e">
@@ -8603,7 +8599,7 @@
     <row r="24" spans="1:24" ht="21">
       <c r="A24" s="30"/>
       <c r="B24" s="198" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24" s="134"/>
       <c r="D24" s="64" t="s">
@@ -8618,7 +8614,7 @@
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J24" s="43"/>
       <c r="K24" s="44" t="e">
@@ -8746,7 +8742,7 @@
       <c r="G26" s="196"/>
       <c r="H26" s="51"/>
       <c r="I26" s="53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="55" t="e">
@@ -8820,7 +8816,7 @@
       </c>
       <c r="H27" s="51"/>
       <c r="I27" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J27" s="43"/>
       <c r="K27" s="44" t="e">
@@ -8878,7 +8874,7 @@
       <c r="G28" s="196"/>
       <c r="H28" s="51"/>
       <c r="I28" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J28" s="43"/>
       <c r="K28" s="44" t="e">
@@ -9006,7 +9002,7 @@
       <c r="G30" s="196"/>
       <c r="H30" s="51"/>
       <c r="I30" s="42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J30" s="43"/>
       <c r="K30" s="44" t="e">
@@ -9134,7 +9130,7 @@
       <c r="G32" s="196"/>
       <c r="H32" s="51"/>
       <c r="I32" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J32" s="43"/>
       <c r="K32" s="44" t="e">
@@ -9204,7 +9200,7 @@
       </c>
       <c r="H33" s="51"/>
       <c r="I33" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J33" s="43"/>
       <c r="K33" s="44" t="e">
@@ -9332,7 +9328,7 @@
       </c>
       <c r="H35" s="51"/>
       <c r="I35" s="53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J35" s="54"/>
       <c r="K35" s="55" t="e">
@@ -9464,7 +9460,7 @@
       </c>
       <c r="H37" s="51"/>
       <c r="I37" s="53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J37" s="54"/>
       <c r="K37" s="55" t="e">
@@ -9654,7 +9650,7 @@
       <c r="G40" s="196"/>
       <c r="H40" s="51"/>
       <c r="I40" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J40" s="43"/>
       <c r="K40" s="44" t="e">
@@ -9724,7 +9720,7 @@
       </c>
       <c r="H41" s="51"/>
       <c r="I41" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J41" s="43"/>
       <c r="K41" s="44" t="e">
@@ -9782,7 +9778,7 @@
       <c r="G42" s="196"/>
       <c r="H42" s="51"/>
       <c r="I42" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J42" s="43"/>
       <c r="K42" s="44" t="e">
@@ -9852,7 +9848,7 @@
       </c>
       <c r="H43" s="51"/>
       <c r="I43" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J43" s="43"/>
       <c r="K43" s="44" t="e">
@@ -9910,7 +9906,7 @@
       <c r="G44" s="196"/>
       <c r="H44" s="51"/>
       <c r="I44" s="42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J44" s="43"/>
       <c r="K44" s="44" t="e">
@@ -9980,7 +9976,7 @@
       </c>
       <c r="H45" s="51"/>
       <c r="I45" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J45" s="43"/>
       <c r="K45" s="44" t="e">
@@ -10038,7 +10034,7 @@
       <c r="G46" s="196"/>
       <c r="H46" s="51"/>
       <c r="I46" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J46" s="43"/>
       <c r="K46" s="44" t="e">
@@ -10166,7 +10162,7 @@
       <c r="G48" s="196"/>
       <c r="H48" s="51"/>
       <c r="I48" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J48" s="43"/>
       <c r="K48" s="44" t="e">
@@ -10236,7 +10232,7 @@
       </c>
       <c r="H49" s="51"/>
       <c r="I49" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J49" s="43"/>
       <c r="K49" s="44" t="e">
@@ -10294,7 +10290,7 @@
       <c r="G50" s="196"/>
       <c r="H50" s="51"/>
       <c r="I50" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J50" s="43"/>
       <c r="K50" s="44" t="e">
@@ -10364,7 +10360,7 @@
       </c>
       <c r="H51" s="51"/>
       <c r="I51" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J51" s="43"/>
       <c r="K51" s="44" t="e">
@@ -10422,7 +10418,7 @@
       <c r="G52" s="196"/>
       <c r="H52" s="51"/>
       <c r="I52" s="42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J52" s="43"/>
       <c r="K52" s="44" t="e">
@@ -10492,7 +10488,7 @@
       </c>
       <c r="H53" s="51"/>
       <c r="I53" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J53" s="43"/>
       <c r="K53" s="44" t="e">
@@ -10620,7 +10616,7 @@
       </c>
       <c r="H55" s="51"/>
       <c r="I55" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J55" s="43"/>
       <c r="K55" s="44" t="e">
@@ -10678,7 +10674,7 @@
       <c r="G56" s="196"/>
       <c r="H56" s="51"/>
       <c r="I56" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J56" s="43"/>
       <c r="K56" s="44" t="e">
@@ -10748,7 +10744,7 @@
       </c>
       <c r="H57" s="51"/>
       <c r="I57" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J57" s="43"/>
       <c r="K57" s="44" t="e">
@@ -10876,7 +10872,7 @@
       </c>
       <c r="H59" s="51"/>
       <c r="I59" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J59" s="43"/>
       <c r="K59" s="44" t="e">
@@ -11004,7 +11000,7 @@
       </c>
       <c r="H61" s="51"/>
       <c r="I61" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J61" s="43"/>
       <c r="K61" s="44" t="e">
@@ -11062,7 +11058,7 @@
       <c r="G62" s="196"/>
       <c r="H62" s="51"/>
       <c r="I62" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J62" s="43"/>
       <c r="K62" s="44" t="e">
@@ -11190,7 +11186,7 @@
       <c r="G64" s="196"/>
       <c r="H64" s="51"/>
       <c r="I64" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J64" s="43"/>
       <c r="K64" s="44" t="e">
@@ -11533,7 +11529,7 @@
       <formula1>"Turtwig,Chimchar,Piplup"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J47" xr:uid="{00000000-0002-0000-0200-000010000000}">
-      <formula1>"Mr. Mime,Floatzel,Shellos,Magikarp,Finneon,Heracross,Wurmple,Burmy,Combee,Cherubi"</formula1>
+      <formula1>"Mr-Mime,Floatzel,Shellos,Magikarp,Finneon,Heracross,Wurmple,Burmy,Combee,Cherubi"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J28" xr:uid="{00000000-0002-0000-0200-000011000000}">
       <formula1>"Eevee"</formula1>
@@ -11653,13 +11649,13 @@
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="F2" s="76" t="s">
         <v>233</v>
-      </c>
-      <c r="F2" s="76" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="3" spans="2:11">
@@ -11667,1537 +11663,1537 @@
         <v>182</v>
       </c>
       <c r="C3" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="E3" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="F3" s="76" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="G3" s="76" t="s">
         <v>238</v>
-      </c>
-      <c r="G3" s="76" t="s">
-        <v>239</v>
       </c>
       <c r="J3" s="76" t="s">
         <v>182</v>
       </c>
       <c r="K3" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" s="76" t="s">
+      <c r="E4" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" s="76" t="s">
         <v>241</v>
       </c>
-      <c r="E4" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F4" s="76" t="s">
-        <v>242</v>
-      </c>
       <c r="G4" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="J4" s="76" t="s">
         <v>239</v>
       </c>
-      <c r="J4" s="76" t="s">
-        <v>240</v>
-      </c>
       <c r="K4" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="76" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D5" s="76" t="s">
+      <c r="E5" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="76" t="s">
         <v>244</v>
       </c>
-      <c r="E5" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F5" s="76" t="s">
-        <v>245</v>
-      </c>
       <c r="G5" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J5" s="76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K5" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="76" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="76" t="s">
+      <c r="E6" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="76" t="s">
         <v>247</v>
       </c>
-      <c r="E6" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F6" s="76" t="s">
-        <v>248</v>
-      </c>
       <c r="G6" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J6" s="76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K6" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" s="76" t="s">
+      <c r="E7" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" s="76" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F7" s="76" t="s">
-        <v>251</v>
-      </c>
       <c r="G7" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J7" s="76" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K7" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="C8" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D8" s="76" t="s">
+      <c r="E8" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F8" s="76" t="s">
-        <v>254</v>
-      </c>
       <c r="G8" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J8" s="76" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K8" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="76" t="s">
         <v>255</v>
       </c>
-      <c r="C9" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D9" s="76" t="s">
+      <c r="E9" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F9" s="76" t="s">
         <v>256</v>
       </c>
-      <c r="E9" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F9" s="76" t="s">
-        <v>257</v>
-      </c>
       <c r="G9" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J9" s="76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K9" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="76" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="C10" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" s="76" t="s">
+      <c r="E10" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="76" t="s">
         <v>259</v>
       </c>
-      <c r="E10" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>260</v>
-      </c>
       <c r="G10" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J10" s="76" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K10" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="76" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="76" t="s">
         <v>261</v>
       </c>
-      <c r="C11" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D11" s="76" t="s">
+      <c r="E11" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="E11" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F11" s="76" t="s">
-        <v>263</v>
-      </c>
       <c r="G11" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J11" s="76" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K11" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="76" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="C12" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D12" s="76" t="s">
+      <c r="E12" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" s="76" t="s">
         <v>265</v>
       </c>
-      <c r="E12" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F12" s="76" t="s">
-        <v>266</v>
-      </c>
       <c r="G12" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J12" s="76" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K12" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="C13" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D13" s="76" t="s">
+      <c r="E13" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="76" t="s">
         <v>268</v>
       </c>
-      <c r="E13" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F13" s="76" t="s">
-        <v>269</v>
-      </c>
       <c r="G13" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J13" s="76" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K13" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="76" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E14" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="76" t="s">
         <v>270</v>
       </c>
-      <c r="C14" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F14" s="76" t="s">
-        <v>271</v>
-      </c>
       <c r="G14" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J14" s="76" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K14" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E15" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="C15" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E15" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F15" s="76" t="s">
-        <v>273</v>
-      </c>
       <c r="G15" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J15" s="76" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K15" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="76" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E16" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F16" s="76" t="s">
         <v>274</v>
       </c>
-      <c r="C16" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F16" s="76" t="s">
-        <v>275</v>
-      </c>
       <c r="G16" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J16" s="76" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K16" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" s="76" t="s">
+        <v>275</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E17" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="76" t="s">
         <v>276</v>
       </c>
-      <c r="C17" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E17" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F17" s="76" t="s">
-        <v>277</v>
-      </c>
       <c r="G17" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J17" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K17" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="76" t="s">
+        <v>236</v>
+      </c>
+      <c r="F18" s="76" t="s">
         <v>278</v>
       </c>
-      <c r="C18" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E18" s="76" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="76" t="s">
-        <v>279</v>
-      </c>
       <c r="G18" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J18" s="76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K18" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="76" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F19" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="C19" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F19" s="76" t="s">
-        <v>281</v>
-      </c>
       <c r="G19" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J19" s="76" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K19" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="76" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F20" s="76" t="s">
         <v>282</v>
       </c>
-      <c r="C20" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F20" s="76" t="s">
-        <v>283</v>
-      </c>
       <c r="G20" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J20" s="76" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K20" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="76" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F21" s="76" t="s">
         <v>284</v>
       </c>
-      <c r="C21" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F21" s="76" t="s">
-        <v>285</v>
-      </c>
       <c r="G21" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J21" s="76" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="76" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F22" s="76" t="s">
         <v>286</v>
       </c>
-      <c r="C22" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F22" s="76" t="s">
-        <v>287</v>
-      </c>
       <c r="G22" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J22" s="76" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K22" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" s="76" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="C23" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F23" s="76" t="s">
-        <v>289</v>
-      </c>
       <c r="G23" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J23" s="76" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K23" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="76" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F24" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="C24" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F24" s="76" t="s">
-        <v>291</v>
-      </c>
       <c r="G24" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J24" s="76" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K24" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="76" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F25" s="76" t="s">
         <v>292</v>
       </c>
-      <c r="C25" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F25" s="76" t="s">
-        <v>293</v>
-      </c>
       <c r="G25" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J25" s="76" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K25" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="76" t="s">
+        <v>293</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="76" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F26" s="76" t="s">
-        <v>295</v>
-      </c>
       <c r="G26" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J26" s="76" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K26" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="C27" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F27" s="76" t="s">
         <v>296</v>
       </c>
-      <c r="C27" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F27" s="76" t="s">
-        <v>297</v>
-      </c>
       <c r="G27" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J27" s="76" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K27" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" s="76" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F28" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="C28" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F28" s="76" t="s">
-        <v>299</v>
-      </c>
       <c r="G28" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J28" s="76" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K28" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" s="76" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F29" s="76" t="s">
         <v>300</v>
       </c>
-      <c r="C29" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F29" s="76" t="s">
-        <v>301</v>
-      </c>
       <c r="G29" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J29" s="76" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K29" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" s="76" t="s">
+        <v>301</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F30" s="76" t="s">
         <v>302</v>
       </c>
-      <c r="C30" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F30" s="76" t="s">
-        <v>303</v>
-      </c>
       <c r="G30" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J30" s="76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K30" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="76" t="s">
+        <v>303</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" s="76" t="s">
         <v>304</v>
       </c>
-      <c r="C31" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F31" s="76" t="s">
-        <v>305</v>
-      </c>
       <c r="G31" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J31" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K31" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" s="76" t="s">
+        <v>305</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F32" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="C32" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F32" s="76" t="s">
-        <v>307</v>
-      </c>
       <c r="G32" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J32" s="76" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K32" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" s="76" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F33" s="76" t="s">
         <v>308</v>
       </c>
-      <c r="C33" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F33" s="76" t="s">
-        <v>309</v>
-      </c>
       <c r="G33" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J33" s="76" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K33" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="76" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F34" s="76" t="s">
         <v>310</v>
       </c>
-      <c r="C34" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>311</v>
-      </c>
       <c r="G34" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J34" s="76" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K34" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="2:11">
       <c r="B35" s="76" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="76" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F35" s="76" t="s">
-        <v>313</v>
-      </c>
       <c r="G35" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J35" s="76" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K35" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="2:11">
       <c r="B36" s="76" t="s">
+        <v>313</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36" s="76" t="s">
         <v>314</v>
       </c>
-      <c r="C36" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F36" s="76" t="s">
-        <v>315</v>
-      </c>
       <c r="G36" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J36" s="76" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K36" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="76" t="s">
+        <v>315</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F37" s="76" t="s">
         <v>316</v>
       </c>
-      <c r="C37" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>317</v>
-      </c>
       <c r="G37" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J37" s="76" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K37" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="2:11">
       <c r="B38" s="76" t="s">
+        <v>317</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F38" s="76" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>319</v>
-      </c>
       <c r="G38" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J38" s="76" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K38" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="2:11">
       <c r="B39" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="76" t="s">
         <v>320</v>
       </c>
-      <c r="C39" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>321</v>
-      </c>
       <c r="G39" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J39" s="76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K39" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="2:11">
       <c r="B40" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F40" s="76" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>323</v>
-      </c>
       <c r="G40" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J40" s="76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K40" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="2:11">
       <c r="B41" s="76" t="s">
+        <v>323</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F41" s="76" t="s">
         <v>324</v>
       </c>
-      <c r="C41" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>325</v>
-      </c>
       <c r="G41" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J41" s="76" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K41" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="2:11">
       <c r="B42" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="C42" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F42" s="76" t="s">
         <v>326</v>
       </c>
-      <c r="C42" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F42" s="76" t="s">
-        <v>327</v>
-      </c>
       <c r="G42" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J42" s="76" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K42" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="2:11">
       <c r="B43" s="76" t="s">
+        <v>327</v>
+      </c>
+      <c r="C43" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F43" s="76" t="s">
         <v>328</v>
       </c>
-      <c r="C43" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="F43" s="76" t="s">
-        <v>329</v>
-      </c>
       <c r="G43" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J43" s="76" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K43" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="2:11">
       <c r="C44" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="G44" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="J44" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="F44" s="76" t="s">
-        <v>330</v>
-      </c>
-      <c r="G44" s="76" t="s">
-        <v>239</v>
-      </c>
-      <c r="J44" s="76" t="s">
+      <c r="K44" s="76" t="s">
         <v>236</v>
-      </c>
-      <c r="K44" s="76" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="45" spans="2:11">
       <c r="C45" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F45" s="76" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G45" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J45" s="76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K45" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="C46" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F46" s="76" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G46" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J46" s="76" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K46" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="2:11">
       <c r="C47" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F47" s="76" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G47" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J47" s="76" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K47" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="2:11">
       <c r="C48" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F48" s="76" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G48" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J48" s="76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K48" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="3:11">
       <c r="C49" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F49" s="76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G49" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J49" s="76" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K49" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="3:11">
       <c r="C50" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F50" s="76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G50" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J50" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K50" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="3:11">
       <c r="C51" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G51" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J51" s="76" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K51" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="3:11">
       <c r="C52" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G52" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J52" s="76" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K52" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="3:11">
       <c r="C53" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G53" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J53" s="76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K53" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="3:11">
       <c r="C54" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G54" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J54" s="76" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K54" s="76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="3:11">
       <c r="C55" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G55" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J55" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="K55" s="76" t="s">
         <v>238</v>
-      </c>
-      <c r="K55" s="76" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="56" spans="3:11">
       <c r="C56" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G56" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J56" s="76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K56" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="3:11">
       <c r="G57" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J57" s="76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K57" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="3:11">
       <c r="G58" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J58" s="76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K58" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="3:11">
       <c r="G59" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J59" s="76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K59" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="3:11">
       <c r="G60" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J60" s="76" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K60" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="3:11">
       <c r="G61" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J61" s="76" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K61" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="3:11">
       <c r="G62" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J62" s="76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K62" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="3:11">
       <c r="G63" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J63" s="76" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K63" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="3:11">
       <c r="G64" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J64" s="76" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K64" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="7:11">
       <c r="G65" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J65" s="76" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K65" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="7:11">
       <c r="G66" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J66" s="76" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K66" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="7:11">
       <c r="G67" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J67" s="76" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K67" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="7:11">
       <c r="G68" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J68" s="76" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K68" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="7:11">
       <c r="G69" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J69" s="76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K69" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="7:11">
       <c r="G70" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J70" s="76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K70" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="7:11">
       <c r="G71" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J71" s="76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K71" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="7:11">
       <c r="G72" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J72" s="76" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K72" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="7:11">
       <c r="G73" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J73" s="76" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K73" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="7:11">
       <c r="G74" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J74" s="76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K74" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="7:11">
       <c r="G75" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J75" s="76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K75" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="7:11">
       <c r="G76" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J76" s="76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K76" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77" spans="7:11">
       <c r="G77" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J77" s="76" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K77" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="7:11">
       <c r="G78" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J78" s="76" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K78" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="7:11">
       <c r="J79" s="76" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K79" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="7:11">
       <c r="J80" s="76" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K80" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="10:11">
       <c r="J81" s="76" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K81" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="10:11">
       <c r="J82" s="76" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K82" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="10:11">
       <c r="J83" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K83" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="10:11">
       <c r="J84" s="76" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K84" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="10:11">
       <c r="J85" s="76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K85" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="10:11">
       <c r="J86" s="76" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K86" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="10:11">
       <c r="J87" s="76" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K87" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="10:11">
       <c r="J88" s="76" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K88" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="10:11">
       <c r="J89" s="76" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K89" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="10:11">
       <c r="J90" s="76" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K90" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="10:11">
       <c r="J91" s="76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K91" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="10:11">
       <c r="J92" s="76" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K92" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="10:11">
       <c r="J93" s="76" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K93" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="10:11">
       <c r="J94" s="76" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K94" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="10:11">
       <c r="J95" s="76" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K95" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="96" spans="10:11">
       <c r="J96" s="76" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K96" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="10:11">
       <c r="J97" s="76" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K97" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="10:11">
       <c r="J98" s="76" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K98" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="10:11">
       <c r="J99" s="76" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K99" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="10:11">
       <c r="J100" s="76" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K100" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="10:11">
       <c r="J101" s="76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K101" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="10:11">
       <c r="J102" s="76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K102" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -13224,11 +13220,11 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="220" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B1" s="129"/>
       <c r="C1" s="213" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" s="221">
         <f>SUM(B6:B13)</f>
@@ -13261,14 +13257,14 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B6" s="80">
         <f>C56</f>
         <v>0</v>
       </c>
       <c r="C6" s="213" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D6" s="221" t="str">
         <f>IF(B18="YES", "YES", "NO")</f>
@@ -13277,7 +13273,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="81" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B7" s="82">
         <f>C65</f>
@@ -13288,7 +13284,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="83" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B8" s="60">
         <f>C16</f>
@@ -13299,7 +13295,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="83" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B9" s="60">
         <f>C25</f>
@@ -13310,14 +13306,14 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B10" s="60">
         <f>C32</f>
         <v>0</v>
       </c>
       <c r="C10" s="213" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D10" s="216">
         <f>IF(D6="YES",(D1*1.5),D1)</f>
@@ -13326,7 +13322,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B11" s="60">
         <f>C42</f>
@@ -13337,7 +13333,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="83" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B12" s="60">
         <f>C47</f>
@@ -13348,7 +13344,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B13" s="85">
         <f>C53</f>
@@ -13365,7 +13361,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="201" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B15" s="202"/>
       <c r="C15" s="202"/>
@@ -13398,7 +13394,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="88" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B18" s="89" t="str">
         <f>IF(Tracker!C14=TRUE, "YES", "NO")</f>
@@ -13409,7 +13405,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="88" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B19" s="89" t="str">
         <f>IF(Tracker!C15=TRUE, "YES", "NO")</f>
@@ -13420,7 +13416,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="88" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B20" s="89" t="str">
         <f>IF(Tracker!C16=TRUE, "YES", "NO")</f>
@@ -13431,7 +13427,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="88" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B21" s="89" t="str">
         <f>IF(Tracker!C17=TRUE, "YES", "NO")</f>
@@ -13442,7 +13438,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="88" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B22" s="89" t="str">
         <f>IF(Tracker!C18=TRUE, "YES", "NO")</f>
@@ -13467,7 +13463,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="90" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B25" s="91" t="str">
         <f>IF(Tracker!C21=TRUE, "40", "0")</f>
@@ -13481,7 +13477,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B26" s="91" t="str">
         <f>IF(Tracker!C22=TRUE, "40", "0")</f>
@@ -13492,7 +13488,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="92" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B27" s="91" t="str">
         <f>IF(Tracker!C23=TRUE, "40", "0")</f>
@@ -13503,7 +13499,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="92" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B28" s="91" t="str">
         <f>IF(Tracker!C24=TRUE, "40", "0")</f>
@@ -13514,7 +13510,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="92" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B29" s="91" t="str">
         <f>IF(Tracker!C25=TRUE, "40", "0")</f>
@@ -13531,7 +13527,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="201" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B31" s="202"/>
       <c r="C31" s="202"/>
@@ -13586,7 +13582,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="95" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B36" s="94" t="str">
         <f>IF(Tracker!G7=TRUE, "60", "0")</f>
@@ -13644,7 +13640,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="98" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B42" s="99" t="str">
         <f>IF(Tracker!C28=TRUE, "20", "0")</f>
@@ -13658,7 +13654,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="98" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B43" s="99" t="str">
         <f>IF(Tracker!C29=TRUE, "20", "0")</f>
@@ -13669,7 +13665,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B44" s="99" t="str">
         <f>IF(Tracker!C30=TRUE, "20", "0")</f>
@@ -13686,7 +13682,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="201" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B46" s="202"/>
       <c r="C46" s="202"/>
@@ -13747,7 +13743,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="201" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B52" s="202"/>
       <c r="C52" s="202"/>
@@ -13775,7 +13771,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="201" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B55" s="202"/>
       <c r="C55" s="202"/>
@@ -13783,7 +13779,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="209" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B56" s="139"/>
       <c r="C56" s="212">
@@ -13794,7 +13790,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="107" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B57" s="108">
         <f>'Team &amp; Encounters'!C21</f>
@@ -13805,7 +13801,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="107" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B58" s="108">
         <f>'Team &amp; Encounters'!C22</f>
@@ -13816,7 +13812,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B59" s="108">
         <f>'Team &amp; Encounters'!C23</f>
@@ -13827,7 +13823,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="107" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B60" s="108">
         <f>'Team &amp; Encounters'!E21</f>
@@ -13838,7 +13834,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="107" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B61" s="108">
         <f>'Team &amp; Encounters'!E22</f>
@@ -13849,7 +13845,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="107" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B62" s="108">
         <f>'Team &amp; Encounters'!E23</f>
@@ -13866,7 +13862,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="201" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B64" s="202"/>
       <c r="C64" s="202"/>
@@ -13874,7 +13870,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="204" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B65" s="139"/>
       <c r="C65" s="205">
@@ -13885,7 +13881,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="109" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B66" s="110">
         <f>COUNTIF(Tracker!J13:J70, "F")</f>
@@ -13896,7 +13892,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="109" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B67" s="110">
         <f>COUNTIF(Tracker!J13:J70, "P")</f>
@@ -13975,7 +13971,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="13.15">
       <c r="A1" s="232" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B1" s="156"/>
       <c r="C1" s="156"/>
@@ -14005,7 +14001,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>45</v>
@@ -14018,7 +14014,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G2" s="114">
         <v>5</v>
@@ -14051,7 +14047,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>48</v>
@@ -14064,7 +14060,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F3" s="64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G3" s="114">
         <v>8</v>
@@ -14097,7 +14093,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>51</v>
@@ -14110,7 +14106,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G4" s="114">
         <v>7</v>
@@ -14120,7 +14116,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J4" s="114">
         <v>7</v>
@@ -14147,7 +14143,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>54</v>
@@ -14160,7 +14156,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F5" s="64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G5" s="114">
         <v>6</v>
@@ -14170,7 +14166,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I5" s="64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J5" s="114">
         <v>8</v>
@@ -14190,7 +14186,7 @@
     </row>
     <row r="6" spans="1:22" ht="72.75" customHeight="1">
       <c r="A6" s="223" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B6" s="156"/>
       <c r="C6" s="156"/>
@@ -14216,7 +14212,7 @@
     </row>
     <row r="7" spans="1:22" ht="13.15">
       <c r="A7" s="233" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B7" s="156"/>
       <c r="C7" s="156"/>
@@ -14246,20 +14242,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B8" s="115" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C8" s="115" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="116" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E8" s="113" t="e">
         <f t="shared" ref="E8:E11" ca="1" si="5">_xludf.image("http://play.pokemonshowdown.com/sprites/gen5/"&amp;LOWER(F8)&amp;".png", 3)</f>
         <v>#NAME?</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G8" s="114">
         <v>11</v>
@@ -14269,7 +14265,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I8" s="64" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J8" s="114">
         <v>11</v>
@@ -14293,7 +14289,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>61</v>
@@ -14306,7 +14302,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G9" s="114">
         <v>15</v>
@@ -14316,7 +14312,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J9" s="114">
         <v>17</v>
@@ -14343,7 +14339,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B10" s="115" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C10" s="115" t="s">
         <v>64</v>
@@ -14356,7 +14352,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G10" s="114">
         <v>8</v>
@@ -14366,7 +14362,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J10" s="114">
         <v>10</v>
@@ -14376,7 +14372,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M10" s="114">
         <v>12</v>
@@ -14386,7 +14382,7 @@
         <v>#NAME?</v>
       </c>
       <c r="O10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P10" s="114">
         <v>12</v>
@@ -14396,7 +14392,7 @@
         <v>#NAME?</v>
       </c>
       <c r="R10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S10" s="114">
         <v>14</v>
@@ -14406,7 +14402,7 @@
         <v>#NAME?</v>
       </c>
       <c r="U10" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V10" s="114">
         <v>16</v>
@@ -14418,7 +14414,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B11" s="115" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C11" s="115" t="s">
         <v>67</v>
@@ -14431,7 +14427,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F11" s="64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G11" s="114">
         <v>19</v>
@@ -14454,7 +14450,7 @@
     </row>
     <row r="12" spans="1:22" ht="75" customHeight="1">
       <c r="A12" s="223" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B12" s="156"/>
       <c r="C12" s="156"/>
@@ -14480,7 +14476,7 @@
     </row>
     <row r="13" spans="1:22" ht="12.75">
       <c r="A13" s="230" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B13" s="156"/>
       <c r="C13" s="156"/>
@@ -14510,7 +14506,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>73</v>
@@ -14523,7 +14519,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G14" s="114">
         <v>21</v>
@@ -14533,7 +14529,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I14" s="64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J14" s="114">
         <v>23</v>
@@ -14560,7 +14556,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>76</v>
@@ -14573,7 +14569,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G15" s="114">
         <v>21</v>
@@ -14606,7 +14602,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>81</v>
@@ -14619,7 +14615,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G16" s="114">
         <v>18</v>
@@ -14629,7 +14625,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I16" s="64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J16" s="114">
         <v>18</v>
@@ -14639,7 +14635,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L16" s="64" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M16" s="114">
         <v>21</v>
@@ -14656,7 +14652,7 @@
     </row>
     <row r="17" spans="1:22" ht="75" customHeight="1">
       <c r="A17" s="223" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="156"/>
       <c r="C17" s="156"/>
@@ -14682,7 +14678,7 @@
     </row>
     <row r="18" spans="1:22" ht="12.75">
       <c r="A18" s="231" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B18" s="122"/>
       <c r="C18" s="122"/>
@@ -14712,7 +14708,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>87</v>
@@ -14725,7 +14721,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F19" s="64" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G19" s="114">
         <v>20</v>
@@ -14735,7 +14731,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I19" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J19" s="114">
         <v>20</v>
@@ -14745,7 +14741,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L19" s="64" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M19" s="114">
         <v>20</v>
@@ -14755,7 +14751,7 @@
         <v>#NAME?</v>
       </c>
       <c r="O19" s="64" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P19" s="114">
         <v>20</v>
@@ -14779,20 +14775,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>90</v>
       </c>
       <c r="D20" s="112" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E20" s="64" t="e">
         <f t="shared" ca="1" si="13"/>
         <v>#NAME?</v>
       </c>
       <c r="F20" s="64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G20" s="114">
         <v>23</v>
@@ -14802,7 +14798,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I20" s="64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J20" s="114">
         <v>23</v>
@@ -14838,7 +14834,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>95</v>
@@ -14851,7 +14847,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G21" s="114">
         <v>19</v>
@@ -14861,7 +14857,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J21" s="114">
         <v>21</v>
@@ -14871,7 +14867,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L21" s="64" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M21" s="114">
         <v>23</v>
@@ -14892,20 +14888,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D22" s="112" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E22" s="64" t="e">
         <f t="shared" ca="1" si="13"/>
         <v>#NAME?</v>
       </c>
       <c r="F22" s="64" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" s="114">
         <v>24</v>
@@ -14915,7 +14911,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I22" s="64" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J22" s="114">
         <v>24</v>
@@ -14942,7 +14938,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>102</v>
@@ -14955,7 +14951,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F23" s="64" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G23" s="114">
         <v>21</v>
@@ -14965,7 +14961,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I23" s="64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J23" s="114">
         <v>24</v>
@@ -14975,7 +14971,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L23" s="64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M23" s="114">
         <v>24</v>
@@ -14992,7 +14988,7 @@
     </row>
     <row r="24" spans="1:22" ht="75" customHeight="1">
       <c r="A24" s="223" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B24" s="156"/>
       <c r="C24" s="156"/>
@@ -15018,7 +15014,7 @@
     </row>
     <row r="25" spans="1:22" ht="12.75">
       <c r="A25" s="222" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B25" s="156"/>
       <c r="C25" s="156"/>
@@ -15048,7 +15044,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C26" s="42" t="s">
         <v>107</v>
@@ -15061,7 +15057,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F26" s="64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G26" s="114">
         <v>26</v>
@@ -15071,7 +15067,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I26" s="64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J26" s="114">
         <v>26</v>
@@ -15098,7 +15094,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>109</v>
@@ -15111,7 +15107,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F27" s="64" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G27" s="114">
         <v>24</v>
@@ -15121,7 +15117,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I27" s="64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J27" s="114">
         <v>24</v>
@@ -15131,7 +15127,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L27" s="64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M27" s="114">
         <v>24</v>
@@ -15152,7 +15148,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C28" s="42" t="s">
         <v>112</v>
@@ -15165,7 +15161,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F28" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G28" s="114">
         <v>25</v>
@@ -15175,7 +15171,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I28" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J28" s="114">
         <v>25</v>
@@ -15185,7 +15181,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L28" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M28" s="114">
         <v>28</v>
@@ -15206,7 +15202,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C29" s="42" t="s">
         <v>114</v>
@@ -15219,7 +15215,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G29" s="114">
         <v>27</v>
@@ -15229,7 +15225,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I29" s="64" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J29" s="114">
         <v>27</v>
@@ -15253,7 +15249,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C30" s="42" t="s">
         <v>118</v>
@@ -15266,7 +15262,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F30" s="64" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G30" s="114">
         <v>28</v>
@@ -15276,7 +15272,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I30" s="64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J30" s="114">
         <v>30</v>
@@ -15296,7 +15292,7 @@
     </row>
     <row r="31" spans="1:22" ht="75" customHeight="1">
       <c r="A31" s="223" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B31" s="156"/>
       <c r="C31" s="156"/>
@@ -15322,7 +15318,7 @@
     </row>
     <row r="32" spans="1:22" ht="12.75">
       <c r="A32" s="227" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B32" s="156"/>
       <c r="C32" s="156"/>
@@ -15352,7 +15348,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>122</v>
@@ -15365,7 +15361,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F33" s="64" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G33" s="114">
         <v>31</v>
@@ -15395,20 +15391,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C34" s="42" t="s">
         <v>124</v>
       </c>
       <c r="D34" s="112" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E34" s="64" t="e">
         <f t="shared" ca="1" si="24"/>
         <v>#NAME?</v>
       </c>
       <c r="F34" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G34" s="114">
         <v>36</v>
@@ -15418,7 +15414,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I34" s="64" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J34" s="114">
         <v>36</v>
@@ -15445,7 +15441,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C35" s="119" t="s">
         <v>128</v>
@@ -15458,7 +15454,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F35" s="64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G35" s="114">
         <v>32</v>
@@ -15468,7 +15464,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I35" s="64" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J35" s="114">
         <v>31</v>
@@ -15478,7 +15474,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L35" s="64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M35" s="114">
         <v>34</v>
@@ -15499,7 +15495,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C36" s="119" t="s">
         <v>130</v>
@@ -15512,7 +15508,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F36" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="114">
         <v>33</v>
@@ -15522,7 +15518,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I36" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J36" s="114">
         <v>33</v>
@@ -15545,7 +15541,7 @@
     </row>
     <row r="37" spans="1:22" ht="75" customHeight="1">
       <c r="A37" s="223" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B37" s="156"/>
       <c r="C37" s="156"/>
@@ -15571,7 +15567,7 @@
     </row>
     <row r="38" spans="1:22" ht="12.75">
       <c r="A38" s="228" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B38" s="156"/>
       <c r="C38" s="156"/>
@@ -15601,7 +15597,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>133</v>
@@ -15614,7 +15610,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F39" s="64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G39" s="114">
         <v>38</v>
@@ -15624,7 +15620,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I39" s="64" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J39" s="114">
         <v>38</v>
@@ -15634,7 +15630,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L39" s="64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M39" s="114">
         <v>40</v>
@@ -15655,7 +15651,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>61</v>
@@ -15668,7 +15664,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F40" s="64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G40" s="114">
         <v>38</v>
@@ -15678,7 +15674,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I40" s="64" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J40" s="114">
         <v>38</v>
@@ -15688,7 +15684,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L40" s="64" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M40" s="114">
         <v>40</v>
@@ -15709,7 +15705,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C41" s="42" t="s">
         <v>136</v>
@@ -15722,7 +15718,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F41" s="64" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G41" s="114">
         <v>39</v>
@@ -15732,7 +15728,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I41" s="64" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J41" s="114">
         <v>40</v>
@@ -15768,7 +15764,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C42" s="42" t="s">
         <v>138</v>
@@ -15781,7 +15777,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F42" s="64" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G42" s="114">
         <v>37</v>
@@ -15791,7 +15787,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I42" s="64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J42" s="114">
         <v>39</v>
@@ -15801,7 +15797,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L42" s="64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M42" s="114">
         <v>39</v>
@@ -15818,7 +15814,7 @@
     </row>
     <row r="43" spans="1:22" ht="75" customHeight="1">
       <c r="A43" s="223" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B43" s="156"/>
       <c r="C43" s="156"/>
@@ -15844,7 +15840,7 @@
     </row>
     <row r="44" spans="1:22" ht="12.75">
       <c r="A44" s="229" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B44" s="156"/>
       <c r="C44" s="156"/>
@@ -15874,7 +15870,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C45" s="119" t="s">
         <v>133</v>
@@ -15887,7 +15883,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F45" s="64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G45" s="114">
         <v>42</v>
@@ -15897,7 +15893,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I45" s="64" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J45" s="114">
         <v>42</v>
@@ -15907,7 +15903,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L45" s="64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M45" s="114">
         <v>44</v>
@@ -15969,7 +15965,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C47" s="119" t="s">
         <v>143</v>
@@ -15982,7 +15978,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F47" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G47" s="114">
         <v>45</v>
@@ -16009,7 +16005,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C48" s="119" t="s">
         <v>145</v>
@@ -16022,7 +16018,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F48" s="64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G48" s="114">
         <v>41</v>
@@ -16032,7 +16028,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I48" s="64" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J48" s="114">
         <v>43</v>
@@ -16042,7 +16038,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L48" s="64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M48" s="114">
         <v>42</v>
@@ -16063,7 +16059,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C49" s="119" t="s">
         <v>146</v>
@@ -16076,7 +16072,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F49" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G49" s="114">
         <v>41</v>
@@ -16086,7 +16082,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I49" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J49" s="114">
         <v>42</v>
@@ -16096,7 +16092,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L49" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M49" s="114">
         <v>41</v>
@@ -16106,7 +16102,7 @@
         <v>#NAME?</v>
       </c>
       <c r="O49" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P49" s="114">
         <v>41</v>
@@ -16124,7 +16120,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C50" s="119" t="s">
         <v>147</v>
@@ -16137,7 +16133,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F50" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G50" s="114">
         <v>43</v>
@@ -16147,7 +16143,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I50" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J50" s="114">
         <v>43</v>
@@ -16157,7 +16153,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L50" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M50" s="114">
         <v>40</v>
@@ -16181,7 +16177,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C51" s="119" t="s">
         <v>148</v>
@@ -16194,7 +16190,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F51" s="64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G51" s="114">
         <v>45</v>
@@ -16204,7 +16200,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I51" s="64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J51" s="114">
         <v>45</v>
@@ -16230,7 +16226,7 @@
     </row>
     <row r="52" spans="1:22" ht="75" customHeight="1">
       <c r="A52" s="223" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B52" s="156"/>
       <c r="C52" s="156"/>
@@ -16256,7 +16252,7 @@
     </row>
     <row r="53" spans="1:22" ht="12.75">
       <c r="A53" s="225" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B53" s="156"/>
       <c r="C53" s="156"/>
@@ -16286,7 +16282,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C54" s="42" t="s">
         <v>151</v>
@@ -16299,7 +16295,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F54" s="64" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G54" s="114">
         <v>43</v>
@@ -16309,7 +16305,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I54" s="64" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J54" s="114">
         <v>46</v>
@@ -16319,7 +16315,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L54" s="64" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M54" s="114">
         <v>46</v>
@@ -16340,7 +16336,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C55" s="42" t="s">
         <v>153</v>
@@ -16353,7 +16349,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F55" s="64" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G55" s="114">
         <v>45</v>
@@ -16363,7 +16359,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I55" s="64" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J55" s="114">
         <v>47</v>
@@ -16393,7 +16389,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B56" s="42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>154</v>
@@ -16406,7 +16402,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F56" s="64" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G56" s="114">
         <v>45</v>
@@ -16416,7 +16412,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I56" s="64" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J56" s="114">
         <v>46</v>
@@ -16426,7 +16422,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L56" s="64" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M56" s="114">
         <v>48</v>
@@ -16450,7 +16446,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>155</v>
@@ -16463,7 +16459,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F57" s="64" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G57" s="114">
         <v>45</v>
@@ -16473,7 +16469,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I57" s="64" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J57" s="114">
         <v>46</v>
@@ -16483,7 +16479,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L57" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M57" s="114">
         <v>48</v>
@@ -16507,7 +16503,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C58" s="42" t="s">
         <v>156</v>
@@ -16520,7 +16516,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F58" s="64" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G58" s="114">
         <v>47</v>
@@ -16530,7 +16526,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I58" s="64" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J58" s="114">
         <v>48</v>
@@ -16554,7 +16550,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C59" s="42" t="s">
         <v>157</v>
@@ -16567,7 +16563,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F59" s="64" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G59" s="114">
         <v>47</v>
@@ -16577,7 +16573,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I59" s="64" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J59" s="114">
         <v>47</v>
@@ -16601,20 +16597,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B60" s="42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>158</v>
       </c>
       <c r="D60" s="112" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E60" s="64" t="e">
         <f t="shared" ca="1" si="38"/>
         <v>#NAME?</v>
       </c>
       <c r="F60" s="64" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G60" s="114">
         <v>50</v>
@@ -16624,7 +16620,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I60" s="64" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J60" s="114">
         <v>50</v>
@@ -16651,7 +16647,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B61" s="42" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C61" s="42" t="s">
         <v>160</v>
@@ -16664,7 +16660,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F61" s="120" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G61" s="114">
         <v>48</v>
@@ -16697,7 +16693,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B62" s="42" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C62" s="42" t="s">
         <v>161</v>
@@ -16710,7 +16706,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F62" s="120" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G62" s="114">
         <v>44</v>
@@ -16720,7 +16716,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I62" s="64" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J62" s="114">
         <v>45</v>
@@ -16730,7 +16726,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L62" s="64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M62" s="114">
         <v>46</v>
@@ -16751,20 +16747,20 @@
         <v>#NAME?</v>
       </c>
       <c r="B63" s="42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C63" s="42" t="s">
         <v>162</v>
       </c>
       <c r="D63" s="112" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E63" s="64" t="e">
         <f t="shared" ca="1" si="38"/>
         <v>#NAME?</v>
       </c>
       <c r="F63" s="64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G63" s="114">
         <v>50</v>
@@ -16774,7 +16770,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I63" s="64" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J63" s="114">
         <v>50</v>
@@ -16801,7 +16797,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B64" s="42" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C64" s="42" t="s">
         <v>164</v>
@@ -16814,7 +16810,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F64" s="120" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G64" s="114">
         <v>47</v>
@@ -16824,7 +16820,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I64" s="64" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J64" s="114">
         <v>48</v>
@@ -16851,7 +16847,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C65" s="42" t="s">
         <v>165</v>
@@ -16864,7 +16860,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F65" s="120" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G65" s="114">
         <v>45</v>
@@ -16874,7 +16870,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I65" s="64" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J65" s="114">
         <v>47</v>
@@ -16901,7 +16897,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B66" s="42" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C66" s="42" t="s">
         <v>166</v>
@@ -16914,7 +16910,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F66" s="120" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G66" s="114">
         <v>46</v>
@@ -16924,7 +16920,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I66" s="64" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J66" s="114">
         <v>46</v>
@@ -16934,7 +16930,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L66" s="64" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M66" s="114">
         <v>46</v>
@@ -16955,7 +16951,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C67" s="42" t="s">
         <v>167</v>
@@ -16968,7 +16964,7 @@
         <v>#NAME?</v>
       </c>
       <c r="F67" s="120" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G67" s="114">
         <v>43</v>
@@ -16978,7 +16974,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I67" s="64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J67" s="114">
         <v>45</v>
@@ -16988,7 +16984,7 @@
         <v>#NAME?</v>
       </c>
       <c r="L67" s="64" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M67" s="114">
         <v>47</v>
@@ -17005,13 +17001,13 @@
     </row>
     <row r="68" spans="1:22" ht="75" customHeight="1">
       <c r="A68" s="223" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B68" s="156"/>
       <c r="C68" s="156"/>
       <c r="D68" s="134"/>
       <c r="E68" s="226" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F68" s="156"/>
       <c r="G68" s="156"/>

</xml_diff>